<commit_message>
damasanji va kami tamizkari
</commit_message>
<xml_diff>
--- a/آردوینو.xlsx
+++ b/آردوینو.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Default.msi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\M\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10050" windowHeight="7575" tabRatio="878" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10050" windowHeight="7575" tabRatio="878"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,10 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="285">
-  <si>
-    <t>معرفی اردینو</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="300">
   <si>
     <t>چشمک زن</t>
   </si>
@@ -127,12 +124,6 @@
     <t xml:space="preserve">شیلد </t>
   </si>
   <si>
-    <t>کتابخونه</t>
-  </si>
-  <si>
-    <t>تابع و نب</t>
-  </si>
-  <si>
     <t>موتور دی سی</t>
   </si>
   <si>
@@ -859,15 +850,9 @@
     <t xml:space="preserve">انواع آن </t>
   </si>
   <si>
-    <t>محوه عملکر</t>
-  </si>
-  <si>
     <t xml:space="preserve">مدار بستن </t>
   </si>
   <si>
-    <t>انالوگ چیست</t>
-  </si>
-  <si>
     <t>analog pins</t>
   </si>
   <si>
@@ -883,15 +868,6 @@
     <t>دماسنجی چیست</t>
   </si>
   <si>
-    <t>انواعش</t>
-  </si>
-  <si>
-    <t>نوع 1</t>
-  </si>
-  <si>
-    <t>نوع 2</t>
-  </si>
-  <si>
     <t>خواندن دما توسط تابع مربوطه</t>
   </si>
   <si>
@@ -902,19 +878,101 @@
   </si>
   <si>
     <t>خاموش کردن رله توسط تابع مربوطه</t>
+  </si>
+  <si>
+    <t>آنالوگ چیست</t>
+  </si>
+  <si>
+    <t>آنالوگ مقاومت متغیر</t>
+  </si>
+  <si>
+    <t xml:space="preserve">آنالوگ دماسنجی </t>
+  </si>
+  <si>
+    <t>تابع و تب</t>
+  </si>
+  <si>
+    <t>کتابخانه</t>
+  </si>
+  <si>
+    <t>ترمیستور</t>
+  </si>
+  <si>
+    <t>ptc - ntc</t>
+  </si>
+  <si>
+    <t>بستن در مدار صرفا به عنوان مقاومت متغیر</t>
+  </si>
+  <si>
+    <t>معادله Steinhart-Hart</t>
+  </si>
+  <si>
+    <t>دیتا شیت ntc10K</t>
+  </si>
+  <si>
+    <t>مدار محاسبه ی دما</t>
+  </si>
+  <si>
+    <t>کد نویسی فرمول ها</t>
+  </si>
+  <si>
+    <t>نمایش در نمایشگر کاراکتری</t>
+  </si>
+  <si>
+    <t>نویز</t>
+  </si>
+  <si>
+    <t>حذف نویز سخت افزاری</t>
+  </si>
+  <si>
+    <t>حذف نویز نرم افزاری</t>
+  </si>
+  <si>
+    <t>حذف نویز ترکیبی</t>
+  </si>
+  <si>
+    <t>فرمول محاسبه ی دما</t>
+  </si>
+  <si>
+    <t>مقایسه ی دو مدل</t>
+  </si>
+  <si>
+    <t>بازه</t>
+  </si>
+  <si>
+    <t>دقت</t>
+  </si>
+  <si>
+    <t>قیمت</t>
+  </si>
+  <si>
+    <t>انواع</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="B Nazanin"/>
+      <charset val="178"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="5">
@@ -955,14 +1013,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1277,10 +1337,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1293,263 +1353,315 @@
     <col min="6" max="6" width="35.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A4" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A6" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B7" s="2"/>
+      <c r="C7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A8" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B8" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A10" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A11" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A12" s="3"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A13" s="3"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A14" s="3"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A19" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A20" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A21" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="B8" t="s">
-        <v>228</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>190</v>
-      </c>
-      <c r="C13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>163</v>
-      </c>
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>164</v>
-      </c>
-      <c r="C15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>160</v>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1557,8 +1669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:C10"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="B4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView rightToLeft="1" topLeftCell="C4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1569,40 +1681,40 @@
   <sheetData>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C4" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -1614,88 +1726,89 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView rightToLeft="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView rightToLeft="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.375" customWidth="1"/>
-    <col min="2" max="2" width="31.875" customWidth="1"/>
-    <col min="3" max="3" width="26.625" customWidth="1"/>
-    <col min="4" max="4" width="35.125" customWidth="1"/>
-    <col min="5" max="5" width="26.875" customWidth="1"/>
+    <col min="1" max="1" width="26.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="31.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="26.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="35.125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="26.875" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B3" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B4" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C1" t="s">
-        <v>242</v>
-      </c>
-      <c r="D1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>232</v>
-      </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B5" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="C2" t="s">
-        <v>243</v>
-      </c>
-      <c r="D2" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B6" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B7" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B8" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B9" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B10" s="2" t="s">
         <v>244</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -1707,8 +1820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView rightToLeft="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView rightToLeft="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1721,40 +1834,40 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" t="s">
         <v>220</v>
-      </c>
-      <c r="C1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D1" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -1767,81 +1880,82 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.375" customWidth="1"/>
-    <col min="2" max="2" width="18.25" customWidth="1"/>
-    <col min="3" max="3" width="17.125" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.5" customWidth="1"/>
-    <col min="6" max="6" width="38.625" customWidth="1"/>
+    <col min="1" max="1" width="14.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.25" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="38.625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B4" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="D4" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="E1" t="s">
-        <v>260</v>
-      </c>
-      <c r="F1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B2" t="s">
-        <v>203</v>
-      </c>
-      <c r="C2" t="s">
-        <v>207</v>
-      </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D5" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="E2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>214</v>
-      </c>
-      <c r="B3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C3" t="s">
-        <v>208</v>
-      </c>
-      <c r="D3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>205</v>
-      </c>
-      <c r="D4" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D5" t="s">
-        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -1864,7 +1978,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -1877,7 +1991,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1892,59 +2006,59 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" t="s">
         <v>146</v>
       </c>
-      <c r="D1" t="s">
-        <v>149</v>
-      </c>
       <c r="E1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1957,7 +2071,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1969,69 +2083,76 @@
     <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B4" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B3" t="s">
-        <v>256</v>
-      </c>
-      <c r="C3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B4" t="s">
-        <v>257</v>
-      </c>
-      <c r="C4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" t="s">
-        <v>159</v>
-      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2056,40 +2177,40 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" t="s">
         <v>151</v>
       </c>
-      <c r="B1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C1" t="s">
-        <v>154</v>
-      </c>
       <c r="D1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" t="s">
         <v>152</v>
       </c>
-      <c r="B2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C2" t="s">
-        <v>155</v>
-      </c>
       <c r="D2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -2101,7 +2222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView rightToLeft="1" zoomScale="246" zoomScaleNormal="246" workbookViewId="0"/>
+    <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2110,7 +2231,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -2120,81 +2241,82 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="23.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.375" customWidth="1"/>
-    <col min="4" max="4" width="22.5" customWidth="1"/>
-    <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="31.375" customWidth="1"/>
-    <col min="7" max="7" width="28.125" customWidth="1"/>
-    <col min="8" max="8" width="25" customWidth="1"/>
+    <col min="1" max="1" width="23.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="24" style="2" customWidth="1"/>
+    <col min="5" max="5" width="31.375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="28.125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="25" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="C4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D4" t="s">
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="C5" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D5" t="s">
-        <v>112</v>
-      </c>
-      <c r="E5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D6" t="s">
-        <v>113</v>
+    </row>
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="C6" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2220,7 +2342,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2232,63 +2354,67 @@
     <col min="5" max="5" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D4" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>72</v>
-      </c>
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2300,96 +2426,100 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D2" t="s">
+      <c r="F3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E4" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E5" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F5" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="G2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F6" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F7" s="5" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F7" t="s">
-        <v>69</v>
-      </c>
+      <c r="G7" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2408,34 +2538,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B1" t="s">
         <v>262</v>
-      </c>
-      <c r="B1" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B3" t="s">
         <v>263</v>
-      </c>
-      <c r="B3" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>261</v>
+      </c>
+      <c r="B4" t="s">
         <v>264</v>
-      </c>
-      <c r="B4" t="s">
-        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -2460,19 +2590,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>93</v>
-      </c>
-      <c r="B1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2495,47 +2625,47 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
         <v>98</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" t="s">
         <v>101</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>102</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>103</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>104</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>105</v>
-      </c>
-      <c r="G1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H1" t="s">
-        <v>107</v>
-      </c>
-      <c r="I1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2572,35 +2702,35 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" t="s">
         <v>181</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>184</v>
       </c>
-      <c r="C1" t="s">
-        <v>187</v>
-      </c>
       <c r="D1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" t="s">
         <v>182</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>185</v>
-      </c>
-      <c r="C2" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" t="s">
         <v>183</v>
-      </c>
-      <c r="B3" t="s">
-        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -2624,29 +2754,29 @@
   <sheetData>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>172</v>
+      </c>
+      <c r="B10" t="s">
         <v>175</v>
       </c>
-      <c r="B10" t="s">
-        <v>178</v>
-      </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>173</v>
+      </c>
+      <c r="B11" t="s">
         <v>176</v>
-      </c>
-      <c r="B11" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2669,40 +2799,43 @@
     <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B3" s="2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>172</v>
-      </c>
-      <c r="B3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>167</v>
-      </c>
-      <c r="B4" t="s">
-        <v>174</v>
-      </c>
+      <c r="C4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2726,46 +2859,46 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3" t="s">
         <v>194</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>197</v>
-      </c>
-      <c r="D3" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2775,51 +2908,120 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="2" width="27.125" customWidth="1"/>
-    <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="26.75" customWidth="1"/>
-    <col min="5" max="5" width="26.625" customWidth="1"/>
+    <col min="1" max="1" width="26.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.75" style="2" customWidth="1"/>
+    <col min="6" max="6" width="26.625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>277</v>
-      </c>
-      <c r="B1" t="s">
-        <v>279</v>
-      </c>
-      <c r="C1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>278</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D3" t="s">
+      <c r="C1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D4" t="s">
+      <c r="C2" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B3" s="2" t="s">
         <v>284</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B4" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B5" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B6" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B7" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B8" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B9" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B10" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B11" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B12" s="2" t="s">
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -2831,52 +3033,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView rightToLeft="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.5" customWidth="1"/>
-    <col min="2" max="2" width="17.875" customWidth="1"/>
-    <col min="3" max="3" width="20.75" customWidth="1"/>
-    <col min="4" max="4" width="22.25" customWidth="1"/>
-    <col min="5" max="5" width="23.75" customWidth="1"/>
+    <col min="1" max="1" width="17.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.75" style="2" customWidth="1"/>
+    <col min="4" max="4" width="22.25" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.75" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>272</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>268</v>
-      </c>
-      <c r="C2" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="C3" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>269</v>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
takmil va namgozari faslha
</commit_message>
<xml_diff>
--- a/آردوینو.xlsx
+++ b/آردوینو.xlsx
@@ -41,9 +41,10 @@
     <sheet name="3 ترانزیستو و رله " sheetId="4" r:id="rId27"/>
     <sheet name="2 چشمک زن " sheetId="3" r:id="rId28"/>
     <sheet name="1 معرفی آردینو " sheetId="2" r:id="rId29"/>
-    <sheet name="پیش نیاز برنامه نویسی" sheetId="26" r:id="rId30"/>
-    <sheet name="پیش نیاز الکتریکی" sheetId="7" r:id="rId31"/>
-    <sheet name="مدار منطقی" sheetId="8" r:id="rId32"/>
+    <sheet name="تمرین فصل 0" sheetId="37" r:id="rId30"/>
+    <sheet name="مدار منطقی" sheetId="8" r:id="rId31"/>
+    <sheet name="پیش نیاز برنامه نویسی" sheetId="26" r:id="rId32"/>
+    <sheet name="پیش نیاز الکتریکی" sheetId="7" r:id="rId33"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="399">
   <si>
     <t>چشمک زن</t>
   </si>
@@ -720,15 +721,6 @@
     <t xml:space="preserve">بازی حافظه </t>
   </si>
   <si>
-    <t>فصل 1</t>
-  </si>
-  <si>
-    <t>فصل 2</t>
-  </si>
-  <si>
-    <t>فصل 3</t>
-  </si>
-  <si>
     <t>سریال قسمت 1</t>
   </si>
   <si>
@@ -954,15 +946,9 @@
     <t xml:space="preserve">آنالوگ رنگ سنجی </t>
   </si>
   <si>
-    <t>فصل 4</t>
-  </si>
-  <si>
     <t>PWM , RGB</t>
   </si>
   <si>
-    <t xml:space="preserve">فصل 5 </t>
-  </si>
-  <si>
     <t>modulation</t>
   </si>
   <si>
@@ -1200,9 +1186,6 @@
     <t>استپر موتور</t>
   </si>
   <si>
-    <t xml:space="preserve">فصل 6 </t>
-  </si>
-  <si>
     <t>سریال قسمت سوم</t>
   </si>
   <si>
@@ -1228,13 +1211,55 @@
   </si>
   <si>
     <t>پیش نیاز برنامه نویسی</t>
+  </si>
+  <si>
+    <t>فاصله سنجی اولتراسونیک</t>
+  </si>
+  <si>
+    <t>فاصله سنجی آی آر</t>
+  </si>
+  <si>
+    <t xml:space="preserve">تمرین فصل 0 </t>
+  </si>
+  <si>
+    <t>آی سی ساعت</t>
+  </si>
+  <si>
+    <t>فصل 0 ( پیش نیازها)</t>
+  </si>
+  <si>
+    <t>فصل 1 (مقدمه)</t>
+  </si>
+  <si>
+    <t>فصل 3 (نمایش داده)</t>
+  </si>
+  <si>
+    <t>فصل 2 (داده)</t>
+  </si>
+  <si>
+    <t>فصل 4 ( AnalogRead )</t>
+  </si>
+  <si>
+    <t>فصل 5 ( Serial &amp; AnalogWrite )</t>
+  </si>
+  <si>
+    <t>فصل 6 (موتورها)</t>
+  </si>
+  <si>
+    <t>فصل 7 (فاصله سنجی و زاویه سنجی)</t>
+  </si>
+  <si>
+    <t>فصل 8 (متفرقه)</t>
+  </si>
+  <si>
+    <t>فصل 9 (ماژول های ارتباطی)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1283,6 +1308,12 @@
       <name val="B Titr"/>
       <charset val="178"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Time "/>
+      <charset val="178"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1317,7 +1348,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1332,6 +1363,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1647,13 +1679,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
     <col min="2" max="2" width="46.25" customWidth="1"/>
@@ -1663,11 +1695,10 @@
     <col min="6" max="6" width="35.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B1" s="2"/>
+    <row r="1" spans="1:5" ht="18">
+      <c r="A1" s="3" t="s">
+        <v>383</v>
+      </c>
       <c r="C1" s="2" t="s">
         <v>157</v>
       </c>
@@ -1678,12 +1709,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>221</v>
+    <row r="2" spans="1:5" ht="18">
+      <c r="A2" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="B2" t="s">
+        <v>389</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
@@ -1695,12 +1726,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
-        <v>80</v>
+    <row r="3" spans="1:5" ht="18">
+      <c r="A3" s="3" t="s">
+        <v>155</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
@@ -1712,9 +1743,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.45">
-      <c r="A4" s="3" t="s">
-        <v>224</v>
+    <row r="4" spans="1:5" ht="18">
+      <c r="A4" s="1" t="s">
+        <v>157</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
@@ -1727,12 +1758,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.45">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
+    <row r="5" spans="1:5" ht="18">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>222</v>
+        <v>390</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>156</v>
@@ -1744,12 +1775,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.45">
-      <c r="A6" s="3" t="s">
-        <v>132</v>
+    <row r="6" spans="1:5" ht="18">
+      <c r="A6" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>13</v>
@@ -1761,9 +1792,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.45">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
+    <row r="7" spans="1:5" ht="18">
+      <c r="A7" s="3" t="s">
+        <v>221</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="4" t="s">
@@ -1776,12 +1807,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.45">
-      <c r="A8" s="1" t="s">
-        <v>225</v>
+    <row r="8" spans="1:5" ht="18">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>223</v>
+        <v>392</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>15</v>
@@ -1793,12 +1824,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.45">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
+    <row r="9" spans="1:5" ht="18">
+      <c r="A9" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>16</v>
@@ -1810,27 +1841,27 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.45">
-      <c r="A10" s="3" t="s">
-        <v>296</v>
+    <row r="10" spans="1:5" ht="18">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.45">
-      <c r="A11" s="3" t="s">
-        <v>274</v>
+    <row r="11" spans="1:5" ht="18">
+      <c r="A11" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>299</v>
+        <v>391</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>26</v>
@@ -1842,12 +1873,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.45">
-      <c r="A12" s="3" t="s">
-        <v>297</v>
+    <row r="12" spans="1:5" ht="18">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>29</v>
@@ -1859,10 +1890,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.45">
-      <c r="A13" s="1" t="s">
-        <v>382</v>
-      </c>
+    <row r="13" spans="1:5" ht="18">
+      <c r="A13" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="B13" s="2"/>
       <c r="C13" s="4" t="s">
         <v>32</v>
       </c>
@@ -1873,12 +1905,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.45">
-      <c r="A14" s="1" t="s">
-        <v>300</v>
+    <row r="14" spans="1:5" ht="18">
+      <c r="A14" s="3" t="s">
+        <v>271</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>301</v>
+        <v>393</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>35</v>
@@ -1890,12 +1922,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.45">
-      <c r="A15" s="1" t="s">
-        <v>298</v>
+    <row r="15" spans="1:5" ht="18">
+      <c r="A15" s="3" t="s">
+        <v>294</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>38</v>
@@ -1907,11 +1939,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.45">
-      <c r="A16" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="B16" s="2"/>
+    <row r="16" spans="1:5" ht="18">
+      <c r="A16" s="1" t="s">
+        <v>376</v>
+      </c>
       <c r="C16" s="2" t="s">
         <v>41</v>
       </c>
@@ -1922,11 +1953,13 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.45">
-      <c r="A17" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B17" s="2"/>
+    <row r="17" spans="1:5" ht="18">
+      <c r="A17" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>394</v>
+      </c>
       <c r="C17" s="4" t="s">
         <v>44</v>
       </c>
@@ -1937,113 +1970,177 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.45">
-      <c r="A18" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B18" s="2"/>
+    <row r="18" spans="1:5" ht="18">
+      <c r="A18" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>381</v>
+      </c>
       <c r="C18" s="4" t="s">
         <v>47</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" ht="18">
       <c r="A19" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>381</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="B19" s="2"/>
       <c r="C19" s="4" t="s">
         <v>92</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" ht="18">
       <c r="A20" s="3" t="s">
-        <v>380</v>
+        <v>158</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" ht="18">
       <c r="A21" s="3" t="s">
-        <v>34</v>
+        <v>159</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" ht="18">
+      <c r="A22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>395</v>
+      </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="8" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="8" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="8" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="8" t="s">
-        <v>155</v>
-      </c>
+    <row r="23" spans="1:5" ht="18">
+      <c r="A23" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" ht="18">
+      <c r="A24" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" ht="18">
+      <c r="A25" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="18">
+      <c r="A26" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="18">
+      <c r="A27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="18">
+      <c r="A28" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="18">
+      <c r="A29" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="18">
+      <c r="A30" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="18">
+      <c r="A31" s="3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="18">
+      <c r="A34" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="8"/>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" location="'4 سریال قسمت اول'!A1" display="سریال قسمت 1"/>
-    <hyperlink ref="A1" location="'1 معرفی آردینو '!A1" display="معرفی آردینو"/>
-    <hyperlink ref="A2" location="'2 چشمک زن '!A1" display="چشمک زن"/>
-    <hyperlink ref="A3" location="'3 ترانزیستو و رله '!A1" display="ترانزیستور و رله ( مفهوم مدار تغذیه و کنترل)"/>
-    <hyperlink ref="A5" location="'5 دکمه'!A1" display="دکمه"/>
-    <hyperlink ref="A6" location="'6 انواع متغیر ها'!A1" display="انواع متغیر"/>
-    <hyperlink ref="A7" location="'7 کیپد'!A1" display="کی پد"/>
-    <hyperlink ref="A8" location="'8 سریال قسمت دوم'!A1" display="سریال قسمت 2"/>
-    <hyperlink ref="A9" location="'9نمایشگر کاراکتری'!A1" display="نمایشگر کاراکتری"/>
-    <hyperlink ref="A10" location="'10 انالوگ مقاومت متغیر'!A1" display="آنالوگ مقاومت متغیر و جوی استیک"/>
-    <hyperlink ref="A11" location="'11 انالوگ دماسنجی'!A1" display="آنالوگ دماسنجی "/>
-    <hyperlink ref="A12" location="'12 آنالوگ نور سنجی'!A1" display="آنالوگ نورسنجی"/>
-    <hyperlink ref="A15" location="'15 آنالوگ رنگ سنجی'!A1" display="آنالوگ رنگ سنجی "/>
-    <hyperlink ref="A13" location="'13سریال قسمت سوم'!A1" display="سریال قسمت سوم"/>
-    <hyperlink ref="A14" location="'14 PWM,RGB'!A1" display="PWM , RGB"/>
-    <hyperlink ref="B3" location="'تمرین فصل 1'!A1" display="تمرین فصل 1"/>
-    <hyperlink ref="B6" location="'تمرین فصل 2'!A1" display="تمرین فصل 2"/>
-    <hyperlink ref="B9" location="'تمرین فصل 3'!A1" display="تمرین فصل 3"/>
-    <hyperlink ref="B12" location="'تمرین فصل 4'!A1" display="تمرین فصل 4"/>
-    <hyperlink ref="B15" location="'تمرین فصل 5'!A1" display="تمرین فصل 5"/>
-    <hyperlink ref="A16" location="'معرفی موتورها'!A1" display="معرفی موتورها"/>
-    <hyperlink ref="A17" location="'موتور دی سی یک'!A1" display="موتور دی سی یک"/>
-    <hyperlink ref="A18" location="'موتور دی سی دو'!A1" display="موتور دی سی دو"/>
-    <hyperlink ref="A19" location="سرو!A1" display="سرو"/>
-    <hyperlink ref="A20" location="استپ!A1" display="استپر موتور"/>
-    <hyperlink ref="A21" location="براشلس!A1" display="براشلس"/>
-    <hyperlink ref="A24" location="'فاصله سنجی'!A1" display="فاصله سنجی "/>
-    <hyperlink ref="A26" location="'حافظه دائمی'!A1" display="حافظه دائمی"/>
-    <hyperlink ref="A28" location="'پیش نیاز الکتریکی'!A1" display="پیش نیاز"/>
-    <hyperlink ref="A29" location="'پیش نیاز برنامه نویسی'!A1" display="پیش نیاز برنامه نویسی"/>
-    <hyperlink ref="A30" location="'مدار منطقی'!A1" display="مدار منطقی"/>
+    <hyperlink ref="A7" location="'4 سریال قسمت اول'!A1" display="سریال قسمت 1"/>
+    <hyperlink ref="A4" location="'1 معرفی آردینو '!A1" display="معرفی آردینو"/>
+    <hyperlink ref="A5" location="'2 چشمک زن '!A1" display="چشمک زن"/>
+    <hyperlink ref="A6" location="'3 ترانزیستو و رله '!A1" display="ترانزیستور و رله ( مفهوم مدار تغذیه و کنترل)"/>
+    <hyperlink ref="A8" location="'5 دکمه'!A1" display="دکمه"/>
+    <hyperlink ref="A9" location="'6 انواع متغیر ها'!A1" display="انواع متغیر"/>
+    <hyperlink ref="A10" location="'7 کیپد'!A1" display="کی پد"/>
+    <hyperlink ref="A11" location="'8 سریال قسمت دوم'!A1" display="سریال قسمت 2"/>
+    <hyperlink ref="A12" location="'9نمایشگر کاراکتری'!A1" display="نمایشگر کاراکتری"/>
+    <hyperlink ref="A13" location="'10 انالوگ مقاومت متغیر'!A1" display="آنالوگ مقاومت متغیر و جوی استیک"/>
+    <hyperlink ref="A14" location="'11 انالوگ دماسنجی'!A1" display="آنالوگ دماسنجی "/>
+    <hyperlink ref="A15" location="'12 آنالوگ نور سنجی'!A1" display="آنالوگ نورسنجی"/>
+    <hyperlink ref="A18" location="'15 آنالوگ رنگ سنجی'!A1" display="آنالوگ رنگ سنجی "/>
+    <hyperlink ref="A16" location="'13سریال قسمت سوم'!A1" display="سریال قسمت سوم"/>
+    <hyperlink ref="A17" location="'14 PWM,RGB'!A1" display="PWM , RGB"/>
+    <hyperlink ref="B6" location="'تمرین فصل 1'!A1" display="تمرین فصل 1"/>
+    <hyperlink ref="B9" location="'تمرین فصل 2'!A1" display="تمرین فصل 2"/>
+    <hyperlink ref="B12" location="'تمرین فصل 3'!A1" display="تمرین فصل 3"/>
+    <hyperlink ref="B15" location="'تمرین فصل 4'!A1" display="تمرین فصل 4"/>
+    <hyperlink ref="B18" location="'تمرین فصل 5'!A1" display="تمرین فصل 5"/>
+    <hyperlink ref="A19" location="'معرفی موتورها'!A1" display="معرفی موتورها"/>
+    <hyperlink ref="A20" location="'موتور دی سی یک'!A1" display="موتور دی سی یک"/>
+    <hyperlink ref="A21" location="'موتور دی سی دو'!A1" display="موتور دی سی دو"/>
+    <hyperlink ref="A22" location="سرو!A1" display="سرو"/>
+    <hyperlink ref="A23" location="استپ!A1" display="استپر موتور"/>
+    <hyperlink ref="A24" location="براشلس!A1" display="براشلس"/>
+    <hyperlink ref="A25" location="'فاصله سنجی'!A1" display="فاصله سنجی "/>
+    <hyperlink ref="A31" location="'حافظه دائمی'!A1" display="حافظه دائمی"/>
+    <hyperlink ref="A1" location="'پیش نیاز الکتریکی'!A1" display="پیش نیاز"/>
+    <hyperlink ref="A2" location="'پیش نیاز برنامه نویسی'!A1" display="پیش نیاز برنامه نویسی"/>
+    <hyperlink ref="A3" location="'مدار منطقی'!A1" display="مدار منطقی"/>
+    <hyperlink ref="B3" location="'تمرین فصل 0'!A1" display="تمرین فصل 0 "/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2058,45 +2155,45 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="80.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="85.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" ht="22.5">
       <c r="A13" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -2115,7 +2212,7 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="17.625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
@@ -2124,34 +2221,34 @@
     <col min="5" max="5" width="51.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E1" t="s">
         <v>332</v>
       </c>
-      <c r="B1" t="s">
-        <v>334</v>
-      </c>
-      <c r="C1" t="s">
-        <v>336</v>
-      </c>
-      <c r="E1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B2" t="s">
+        <v>330</v>
+      </c>
+      <c r="E2" t="s">
         <v>333</v>
       </c>
-      <c r="B2" t="s">
-        <v>335</v>
-      </c>
-      <c r="E2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:5" ht="22.5">
       <c r="C9" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -2170,7 +2267,7 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="17.25" customWidth="1"/>
     <col min="2" max="2" width="19.75" customWidth="1"/>
@@ -2178,47 +2275,47 @@
     <col min="4" max="4" width="24.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" ht="18">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15">
       <c r="A2" s="4" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18">
       <c r="A3" s="4" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18">
       <c r="A4" s="2" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="22.5">
       <c r="C11" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -2237,7 +2334,7 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="28.125" customWidth="1"/>
     <col min="2" max="2" width="27.875" bestFit="1" customWidth="1"/>
@@ -2248,80 +2345,80 @@
     <col min="7" max="7" width="32.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B1" t="s">
+        <v>352</v>
+      </c>
+      <c r="C1" t="s">
+        <v>361</v>
+      </c>
+      <c r="D1" t="s">
+        <v>364</v>
+      </c>
+      <c r="E1" t="s">
+        <v>356</v>
+      </c>
+      <c r="F1" t="s">
+        <v>366</v>
+      </c>
+      <c r="G1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B2" t="s">
         <v>353</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D2" t="s">
+        <v>358</v>
+      </c>
+      <c r="E2" t="s">
         <v>357</v>
       </c>
-      <c r="C1" t="s">
-        <v>366</v>
-      </c>
-      <c r="D1" t="s">
-        <v>369</v>
-      </c>
-      <c r="E1" t="s">
-        <v>361</v>
-      </c>
-      <c r="F1" t="s">
-        <v>371</v>
-      </c>
-      <c r="G1" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="F2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>350</v>
+      </c>
+      <c r="B3" t="s">
         <v>354</v>
       </c>
-      <c r="B2" t="s">
-        <v>358</v>
-      </c>
-      <c r="C2" t="s">
-        <v>367</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
         <v>363</v>
       </c>
-      <c r="E2" t="s">
-        <v>362</v>
-      </c>
-      <c r="F2" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="D3" t="s">
+        <v>359</v>
+      </c>
+      <c r="E3" t="s">
+        <v>365</v>
+      </c>
+      <c r="F3" t="s">
         <v>355</v>
       </c>
-      <c r="B3" t="s">
-        <v>359</v>
-      </c>
-      <c r="C3" t="s">
-        <v>368</v>
-      </c>
-      <c r="D3" t="s">
-        <v>364</v>
-      </c>
-      <c r="E3" t="s">
-        <v>370</v>
-      </c>
-      <c r="F3" t="s">
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>351</v>
+      </c>
+      <c r="D4" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>356</v>
-      </c>
-      <c r="D4" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="22.5">
       <c r="B11" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -2340,45 +2437,45 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="75" customWidth="1"/>
     <col min="2" max="2" width="64.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" ht="22.5">
       <c r="A11" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -2397,7 +2494,7 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="28.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.75" customWidth="1"/>
@@ -2406,33 +2503,33 @@
     <col min="5" max="5" width="25.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B1" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="C1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="B2" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="22.5">
       <c r="C9" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -2451,7 +2548,7 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="26.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="28.125" style="2" bestFit="1" customWidth="1"/>
@@ -2462,108 +2559,108 @@
     <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="B3" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>108</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="B4" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="B5" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="B6" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="B7" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B5" s="2" t="s">
+    </row>
+    <row r="8" spans="1:5">
+      <c r="B8" s="2" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B6" s="2" t="s">
+    <row r="9" spans="1:5">
+      <c r="B9" s="2" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B7" s="2" t="s">
+    <row r="10" spans="1:5">
+      <c r="B10" s="2" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B8" s="2" t="s">
+    <row r="11" spans="1:5">
+      <c r="B11" s="2" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B9" s="2" t="s">
+    <row r="12" spans="1:5">
+      <c r="B12" s="2" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B10" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B11" s="2" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B12" s="2" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" ht="22.5">
       <c r="C15" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -2582,7 +2679,7 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="17.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="17.875" style="2" customWidth="1"/>
@@ -2592,24 +2689,24 @@
     <col min="6" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>269</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -2617,25 +2714,25 @@
         <v>112</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="B3" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="B4" s="2" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="22.5" x14ac:dyDescent="0.45">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="22.5">
       <c r="C10" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -2655,60 +2752,60 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="44.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" ht="22.5">
       <c r="A1" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="22.5">
+      <c r="A2" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="B2" s="6"/>
+    </row>
+    <row r="3" spans="1:2" ht="22.5">
+      <c r="A3" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="B3" s="6"/>
+    </row>
+    <row r="4" spans="1:2" ht="22.5">
+      <c r="A4" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B4" s="6"/>
+    </row>
+    <row r="5" spans="1:2" ht="22.5">
+      <c r="A5" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="1:2" ht="22.5">
+      <c r="A6" s="6" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="6" t="s">
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:2" ht="22.5">
+      <c r="A7" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="B2" s="6"/>
-    </row>
-    <row r="3" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="B3" s="6"/>
-    </row>
-    <row r="4" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="B4" s="6"/>
-    </row>
-    <row r="5" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="B5" s="6"/>
-    </row>
-    <row r="6" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="B6" s="6"/>
-    </row>
-    <row r="7" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="6" t="s">
-        <v>248</v>
-      </c>
       <c r="B7" s="6"/>
     </row>
-    <row r="9" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="22.5">
       <c r="B9" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -2728,7 +2825,7 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="26.375" style="2" customWidth="1"/>
     <col min="2" max="2" width="31.875" style="2" customWidth="1"/>
@@ -2738,80 +2835,80 @@
     <col min="6" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="B3" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B3" s="2" t="s">
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="C3" s="2" t="s">
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="B8" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10" s="2" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B4" s="2" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B5" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B6" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B7" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B8" s="2" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B9" s="2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B10" s="2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" ht="22.5">
       <c r="B13" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -2830,61 +2927,61 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" ht="24">
       <c r="A1" s="6" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="24">
       <c r="A2" s="6" t="s">
         <v>177</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="24">
+      <c r="A3" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="24">
+      <c r="A4" s="6" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="6" t="s">
+      <c r="B4" s="7" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="20.25">
+      <c r="B5" s="7" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="20.25">
+      <c r="B6" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B5" s="7" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B6" s="7" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:3" ht="22.5">
       <c r="C9" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -2903,7 +3000,7 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="22.5" customWidth="1"/>
     <col min="2" max="2" width="25.875" bestFit="1" customWidth="1"/>
@@ -2911,7 +3008,7 @@
     <col min="4" max="4" width="46.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>210</v>
       </c>
@@ -2922,10 +3019,10 @@
         <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>211</v>
       </c>
@@ -2936,7 +3033,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>212</v>
       </c>
@@ -2944,14 +3041,14 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="22.5">
       <c r="B13" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -2970,7 +3067,7 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="14.375" style="2" customWidth="1"/>
     <col min="2" max="2" width="18.25" style="2" customWidth="1"/>
@@ -2981,7 +3078,7 @@
     <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>112</v>
       </c>
@@ -2995,13 +3092,13 @@
         <v>204</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>196</v>
       </c>
@@ -3015,10 +3112,10 @@
         <v>205</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>209</v>
       </c>
@@ -3032,7 +3129,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6">
       <c r="B4" s="2" t="s">
         <v>200</v>
       </c>
@@ -3040,14 +3137,14 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6">
       <c r="D5" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" ht="22.5">
       <c r="B13" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -3066,21 +3163,21 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="17.75" customWidth="1"/>
     <col min="2" max="2" width="17.875" customWidth="1"/>
     <col min="3" max="3" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="22.5">
       <c r="B6" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -3099,7 +3196,7 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="19.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.625" customWidth="1"/>
@@ -3109,7 +3206,7 @@
     <col min="7" max="7" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>133</v>
       </c>
@@ -3129,10 +3226,10 @@
         <v>143</v>
       </c>
       <c r="G1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -3143,32 +3240,32 @@
         <v>145</v>
       </c>
       <c r="G2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="B3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="B4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="B5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="B6" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="22.5">
       <c r="B13" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -3187,7 +3284,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
@@ -3196,7 +3293,7 @@
     <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="18">
       <c r="A1" s="2" t="s">
         <v>112</v>
       </c>
@@ -3213,7 +3310,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="18">
       <c r="A2" s="2" t="s">
         <v>113</v>
       </c>
@@ -3228,12 +3325,12 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" ht="18">
       <c r="A3" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>121</v>
@@ -3243,12 +3340,12 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" ht="18">
       <c r="A4" s="2" t="s">
         <v>115</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>122</v>
@@ -3256,7 +3353,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" ht="18">
       <c r="A5" s="2" t="s">
         <v>116</v>
       </c>
@@ -3267,9 +3364,9 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="22.5">
       <c r="C13" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -3288,7 +3385,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
@@ -3296,7 +3393,7 @@
     <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>146</v>
       </c>
@@ -3310,7 +3407,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>147</v>
       </c>
@@ -3324,19 +3421,19 @@
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="22.5">
       <c r="C13" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -3356,19 +3453,19 @@
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="24.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="22.5">
       <c r="B7" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -3387,7 +3484,7 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="23.375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.375" style="2" customWidth="1"/>
@@ -3399,7 +3496,7 @@
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>160</v>
       </c>
@@ -3413,7 +3510,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>85</v>
       </c>
@@ -3427,7 +3524,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>86</v>
       </c>
@@ -3438,7 +3535,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4">
       <c r="C4" s="2" t="s">
         <v>106</v>
       </c>
@@ -3446,7 +3543,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4">
       <c r="C5" s="2" t="s">
         <v>107</v>
       </c>
@@ -3454,14 +3551,14 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4">
       <c r="C6" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" ht="22.5">
       <c r="B11" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -3481,7 +3578,7 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.25" customWidth="1"/>
@@ -3490,7 +3587,7 @@
     <col min="5" max="5" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" ht="18">
       <c r="A1" s="2" t="s">
         <v>123</v>
       </c>
@@ -3504,7 +3601,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" ht="18">
       <c r="A2" s="2" t="s">
         <v>124</v>
       </c>
@@ -3518,7 +3615,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" ht="18">
       <c r="A3" s="2" t="s">
         <v>125</v>
       </c>
@@ -3532,7 +3629,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" ht="18">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>129</v>
@@ -3544,7 +3641,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" ht="18">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>69</v>
@@ -3552,9 +3649,9 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="22.5">
       <c r="B13" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -3573,7 +3670,7 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="14" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.875" style="2" bestFit="1" customWidth="1"/>
@@ -3585,7 +3682,7 @@
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
@@ -3608,7 +3705,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
         <v>55</v>
       </c>
@@ -3622,7 +3719,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7">
       <c r="E3" s="2" t="s">
         <v>57</v>
       </c>
@@ -3633,7 +3730,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7">
       <c r="E4" s="2" t="s">
         <v>58</v>
       </c>
@@ -3644,7 +3741,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7">
       <c r="E5" s="2" t="s">
         <v>59</v>
       </c>
@@ -3653,21 +3750,21 @@
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7">
       <c r="F6" s="4" t="s">
         <v>65</v>
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7">
       <c r="F7" s="4" t="s">
         <v>66</v>
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="22.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" ht="22.5">
       <c r="C10" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -3686,7 +3783,7 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
@@ -3694,50 +3791,50 @@
     <col min="4" max="4" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" ht="18">
       <c r="A1" s="2" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C1" t="s">
         <v>314</v>
       </c>
-      <c r="C1" t="s">
-        <v>319</v>
-      </c>
       <c r="D1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18">
       <c r="A2" s="2" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="C2" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18">
       <c r="A3" s="2" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="C3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="C4" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="22.5">
       <c r="C8" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -3751,49 +3848,151 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="12.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15">
+      <c r="A1" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="22.5">
+      <c r="C4" s="9" t="s">
+        <v>382</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" location="Sheet1!A1" display="صفحه اصلی"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="22.5">
+      <c r="G7" s="9" t="s">
+        <v>382</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G7" location="Sheet1!A1" display="صفحه اصلی"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B1" t="s">
         <v>257</v>
       </c>
-      <c r="B1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B3" t="s">
         <v>258</v>
       </c>
-      <c r="B3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>256</v>
+      </c>
+      <c r="B4" t="s">
         <v>259</v>
       </c>
-      <c r="B4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:4" ht="22.5">
       <c r="D9" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -3804,7 +4003,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -3812,16 +4011,16 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="22.5">
       <c r="A1" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="B1" t="s">
         <v>89</v>
@@ -3836,86 +4035,15 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="22.5">
       <c r="E9" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" location="Sheet1!A1" display="صفحه اصلی"/>
     <hyperlink ref="E9" location="Sheet1!A1" display="صفحه اصلی"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
-  <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H1" t="s">
-        <v>102</v>
-      </c>
-      <c r="I1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>95</v>
-      </c>
-      <c r="H3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="G7" s="9" t="s">
-        <v>388</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G7" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3929,11 +4057,11 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="11" spans="4:4" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="4:4" ht="22.5">
       <c r="D11" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -3952,11 +4080,11 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="10" spans="4:4" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="4:4" ht="22.5">
       <c r="D10" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -3975,14 +4103,14 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>176</v>
       </c>
@@ -3996,7 +4124,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>177</v>
       </c>
@@ -4007,7 +4135,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>178</v>
       </c>
@@ -4015,9 +4143,9 @@
         <v>181</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="22.5">
       <c r="D9" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -4036,13 +4164,13 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="11.875" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>170</v>
       </c>
@@ -4056,7 +4184,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>171</v>
       </c>
@@ -4064,14 +4192,14 @@
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="22.5">
       <c r="D9" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -4090,14 +4218,14 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="18">
       <c r="A1" s="2" t="s">
         <v>161</v>
       </c>
@@ -4108,7 +4236,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" ht="18">
       <c r="A2" s="2" t="s">
         <v>166</v>
       </c>
@@ -4117,7 +4245,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" ht="18">
       <c r="A3" s="2" t="s">
         <v>167</v>
       </c>
@@ -4126,7 +4254,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" ht="18">
       <c r="A4" s="2" t="s">
         <v>162</v>
       </c>
@@ -4135,9 +4263,9 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="10" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="22.5">
       <c r="C10" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -4156,14 +4284,14 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="15.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>186</v>
       </c>
@@ -4177,7 +4305,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="B2" t="s">
         <v>188</v>
       </c>
@@ -4188,7 +4316,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="B3" t="s">
         <v>189</v>
       </c>
@@ -4199,7 +4327,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="B4" t="s">
         <v>190</v>
       </c>
@@ -4207,9 +4335,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="22.5">
       <c r="D12" s="9" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
eslahe faslha, takmile motorha, ezhafe kardan chand tab
</commit_message>
<xml_diff>
--- a/آردوینو.xlsx
+++ b/آردوینو.xlsx
@@ -13,38 +13,49 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="حافظه دائمی" sheetId="34" r:id="rId2"/>
-    <sheet name="فاصله سنجی" sheetId="33" r:id="rId3"/>
-    <sheet name="براشلس" sheetId="17" r:id="rId4"/>
-    <sheet name="استپ" sheetId="16" r:id="rId5"/>
-    <sheet name="سرو" sheetId="14" r:id="rId6"/>
-    <sheet name="موتور دی سی دو" sheetId="13" r:id="rId7"/>
-    <sheet name="موتور دی سی یک" sheetId="12" r:id="rId8"/>
-    <sheet name="معرفی موتورها" sheetId="15" r:id="rId9"/>
-    <sheet name="تمرین فصل 5" sheetId="36" r:id="rId10"/>
-    <sheet name="15 آنالوگ رنگ سنجی" sheetId="29" r:id="rId11"/>
-    <sheet name="14 PWM,RGB" sheetId="32" r:id="rId12"/>
-    <sheet name="13سریال قسمت سوم" sheetId="35" r:id="rId13"/>
-    <sheet name="تمرین فصل 4" sheetId="31" r:id="rId14"/>
-    <sheet name="12 آنالوگ نور سنجی" sheetId="30" r:id="rId15"/>
-    <sheet name="11 انالوگ دماسنجی" sheetId="28" r:id="rId16"/>
-    <sheet name="10 انالوگ مقاومت متغیر" sheetId="27" r:id="rId17"/>
-    <sheet name="تمرین فصل 3" sheetId="25" r:id="rId18"/>
-    <sheet name="9نمایشگر کاراکتری" sheetId="24" r:id="rId19"/>
-    <sheet name="8 سریال قسمت دوم" sheetId="21" r:id="rId20"/>
-    <sheet name="7 کیپد" sheetId="18" r:id="rId21"/>
-    <sheet name="تمرین فصل 2" sheetId="23" r:id="rId22"/>
-    <sheet name="6 انواع متغیر ها" sheetId="10" r:id="rId23"/>
-    <sheet name="5 دکمه" sheetId="9" r:id="rId24"/>
-    <sheet name="4 سریال قسمت اول" sheetId="11" r:id="rId25"/>
-    <sheet name="تمرین فصل 1" sheetId="22" r:id="rId26"/>
-    <sheet name="3 ترانزیستو و رله " sheetId="4" r:id="rId27"/>
-    <sheet name="2 چشمک زن " sheetId="3" r:id="rId28"/>
-    <sheet name="1 معرفی آردینو " sheetId="2" r:id="rId29"/>
-    <sheet name="تمرین فصل 0" sheetId="37" r:id="rId30"/>
-    <sheet name="مدار منطقی" sheetId="8" r:id="rId31"/>
-    <sheet name="پیش نیاز برنامه نویسی" sheetId="26" r:id="rId32"/>
-    <sheet name="پیش نیاز الکتریکی" sheetId="7" r:id="rId33"/>
+    <sheet name="32 SD Card" sheetId="48" r:id="rId2"/>
+    <sheet name=" 31 EEPROM" sheetId="34" r:id="rId3"/>
+    <sheet name="30 Tone" sheetId="47" r:id="rId4"/>
+    <sheet name="29 کاربرد SPI" sheetId="46" r:id="rId5"/>
+    <sheet name="28 SPI" sheetId="45" r:id="rId6"/>
+    <sheet name="27 آی سی ساعت" sheetId="38" r:id="rId7"/>
+    <sheet name=" 26 I2C " sheetId="39" r:id="rId8"/>
+    <sheet name="تمرین فصل 7" sheetId="44" r:id="rId9"/>
+    <sheet name="25 روتاری انکودر" sheetId="43" r:id="rId10"/>
+    <sheet name="24 شافت انکودر" sheetId="42" r:id="rId11"/>
+    <sheet name="23 فاصله سنجی آی آر" sheetId="41" r:id="rId12"/>
+    <sheet name="22 فاصله سنجی اولتراسونیک" sheetId="33" r:id="rId13"/>
+    <sheet name="تمرین فصل 6" sheetId="40" r:id="rId14"/>
+    <sheet name="21 براشلس" sheetId="17" r:id="rId15"/>
+    <sheet name="20 استپ" sheetId="16" r:id="rId16"/>
+    <sheet name="19 سرو" sheetId="14" r:id="rId17"/>
+    <sheet name="18 موتور دی سی دو" sheetId="13" r:id="rId18"/>
+    <sheet name="17 موتور دی سی یک" sheetId="12" r:id="rId19"/>
+    <sheet name="16 معرفی موتورها" sheetId="15" r:id="rId20"/>
+    <sheet name="تمرین فصل 5" sheetId="36" r:id="rId21"/>
+    <sheet name="15 آنالوگ رنگ سنجی" sheetId="29" r:id="rId22"/>
+    <sheet name="14 PWM,RGB" sheetId="32" r:id="rId23"/>
+    <sheet name="13سریال قسمت سوم" sheetId="35" r:id="rId24"/>
+    <sheet name="تمرین فصل 4" sheetId="31" r:id="rId25"/>
+    <sheet name="12 آنالوگ نور سنجی" sheetId="30" r:id="rId26"/>
+    <sheet name="11 انالوگ دماسنجی" sheetId="28" r:id="rId27"/>
+    <sheet name="10 انالوگ مقاومت متغیر" sheetId="27" r:id="rId28"/>
+    <sheet name="تمرین فصل 3" sheetId="25" r:id="rId29"/>
+    <sheet name="9نمایشگر کاراکتری" sheetId="24" r:id="rId30"/>
+    <sheet name="8 سریال قسمت دوم" sheetId="21" r:id="rId31"/>
+    <sheet name="7 کیپد" sheetId="18" r:id="rId32"/>
+    <sheet name="تمرین فصل 2" sheetId="23" r:id="rId33"/>
+    <sheet name="6 انواع متغیر ها" sheetId="10" r:id="rId34"/>
+    <sheet name="5 دکمه" sheetId="9" r:id="rId35"/>
+    <sheet name="4 سریال قسمت اول" sheetId="11" r:id="rId36"/>
+    <sheet name="تمرین فصل 1" sheetId="22" r:id="rId37"/>
+    <sheet name="3 ترانزیستو و رله " sheetId="4" r:id="rId38"/>
+    <sheet name="2 چشمک زن " sheetId="3" r:id="rId39"/>
+    <sheet name="1 معرفی آردینو " sheetId="2" r:id="rId40"/>
+    <sheet name="تمرین فصل 0" sheetId="37" r:id="rId41"/>
+    <sheet name="مدار منطقی" sheetId="8" r:id="rId42"/>
+    <sheet name="پیش نیاز برنامه نویسی" sheetId="26" r:id="rId43"/>
+    <sheet name="پیش نیاز الکتریکی" sheetId="7" r:id="rId44"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -56,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="443">
   <si>
     <t>چشمک زن</t>
   </si>
@@ -1006,9 +1017,6 @@
     <t>pulseIn  دستور</t>
   </si>
   <si>
-    <t>حافظه دائمی</t>
-  </si>
-  <si>
     <t>حافظه دائمی چیست</t>
   </si>
   <si>
@@ -1033,9 +1041,6 @@
     <t>انواع حافظه دائمی</t>
   </si>
   <si>
-    <t>حافظه های جانبی</t>
-  </si>
-  <si>
     <t>سنسور  tctr500</t>
   </si>
   <si>
@@ -1129,9 +1134,6 @@
     <t>String</t>
   </si>
   <si>
-    <t>کاربرد string</t>
-  </si>
-  <si>
     <t>serial.parsefloat</t>
   </si>
   <si>
@@ -1249,17 +1251,204 @@
     <t>فصل 7 (فاصله سنجی و زاویه سنجی)</t>
   </si>
   <si>
-    <t>فصل 8 (متفرقه)</t>
-  </si>
-  <si>
-    <t>فصل 9 (ماژول های ارتباطی)</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve">کاربرد </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>string</t>
+    </r>
+  </si>
+  <si>
+    <t>قطعه کاربردی برای SPI</t>
+  </si>
+  <si>
+    <t>فصل 8 (دیگر ارتباط ها)</t>
+  </si>
+  <si>
+    <t>فصل 9 (متفرقه)</t>
+  </si>
+  <si>
+    <t>فصل 10 (ماژول های ارتباطی)</t>
+  </si>
+  <si>
+    <t>SD Card</t>
+  </si>
+  <si>
+    <t>DS1307</t>
+  </si>
+  <si>
+    <t>کریستال</t>
+  </si>
+  <si>
+    <t>باطری</t>
+  </si>
+  <si>
+    <t>مدار</t>
+  </si>
+  <si>
+    <t>ویژگی های فنی</t>
+  </si>
+  <si>
+    <t>سیم های مورد نیاز</t>
+  </si>
+  <si>
+    <t>محدودیت</t>
+  </si>
+  <si>
+    <t>begin</t>
+  </si>
+  <si>
+    <t>beginTransmission</t>
+  </si>
+  <si>
+    <t>endTransmission</t>
+  </si>
+  <si>
+    <t>available</t>
+  </si>
+  <si>
+    <t>setClock</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="B Nazanin"/>
+        <charset val="178"/>
+      </rPr>
+      <t>کتابخانه</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>Wire</t>
+    </r>
+  </si>
+  <si>
+    <t>مقاومت</t>
+  </si>
+  <si>
+    <t>استپر چیست</t>
+  </si>
+  <si>
+    <t>ساختار درونی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">پین ها </t>
+  </si>
+  <si>
+    <t>کد و مدار</t>
+  </si>
+  <si>
+    <t>تفاوت ها با  A4988</t>
+  </si>
+  <si>
+    <t>کتابخانه Stepper</t>
+  </si>
+  <si>
+    <t>setSpeed</t>
+  </si>
+  <si>
+    <t>step</t>
+  </si>
+  <si>
+    <t>براشلس چیست</t>
+  </si>
+  <si>
+    <t>مزایا و معایب</t>
+  </si>
+  <si>
+    <t>ثابت ولتاژ</t>
+  </si>
+  <si>
+    <t>ثابت گشتاور</t>
+  </si>
+  <si>
+    <t>جریان بدون بار</t>
+  </si>
+  <si>
+    <t>مقاومت ترمینال</t>
+  </si>
+  <si>
+    <t>توان</t>
+  </si>
+  <si>
+    <t>ESC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">مدار </t>
+  </si>
+  <si>
+    <t>تمرین فصل 6</t>
+  </si>
+  <si>
+    <t>تمرین فصل 7</t>
+  </si>
+  <si>
+    <t>کتابخانه SPI</t>
+  </si>
+  <si>
+    <t>beginTransaction</t>
+  </si>
+  <si>
+    <t>SPISettings</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>endTransaction</t>
+  </si>
+  <si>
+    <t>transfer</t>
+  </si>
+  <si>
+    <t>تولید صدا</t>
+  </si>
+  <si>
+    <t>نت ها</t>
+  </si>
+  <si>
+    <t>ملودی</t>
+  </si>
+  <si>
+    <t>دستور tone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1287,13 +1476,6 @@
       <charset val="178"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <scheme val="major"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -1310,9 +1492,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Time "/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="B Nazanin"/>
       <charset val="178"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1346,9 +1548,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1358,12 +1560,15 @@
       <alignment horizontal="right" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1679,13 +1884,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
     <col min="2" max="2" width="46.25" customWidth="1"/>
@@ -1695,9 +1900,9 @@
     <col min="6" max="6" width="35.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>157</v>
@@ -1709,12 +1914,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B2" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
@@ -1726,12 +1931,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18">
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>387</v>
+      <c r="B3" s="7" t="s">
+        <v>384</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
@@ -1743,7 +1948,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18">
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>157</v>
       </c>
@@ -1758,12 +1963,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18">
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>156</v>
@@ -1775,12 +1980,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18">
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>377</v>
+      <c r="B6" s="7" t="s">
+        <v>374</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>13</v>
@@ -1792,7 +1997,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18">
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>221</v>
       </c>
@@ -1807,12 +2012,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18">
+    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>15</v>
@@ -1824,12 +2029,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18">
+    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>378</v>
+      <c r="B9" s="7" t="s">
+        <v>375</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>16</v>
@@ -1841,7 +2046,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18">
+    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1856,12 +2061,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="18">
+    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>222</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>26</v>
@@ -1873,12 +2078,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="18">
+    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>379</v>
+      <c r="B12" s="7" t="s">
+        <v>376</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>29</v>
@@ -1890,7 +2095,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="18">
+    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>293</v>
       </c>
@@ -1905,12 +2110,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="18">
+    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>271</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>35</v>
@@ -1922,12 +2127,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="18">
+    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>380</v>
+      <c r="B15" s="7" t="s">
+        <v>377</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>38</v>
@@ -1939,9 +2144,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="18">
+    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>41</v>
@@ -1953,12 +2158,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="18">
+    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>296</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>44</v>
@@ -1970,12 +2175,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="18">
+    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>381</v>
+      <c r="B18" s="7" t="s">
+        <v>378</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>47</v>
@@ -1985,7 +2190,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="18">
+    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>185</v>
       </c>
@@ -1996,7 +2201,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="18">
+    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>158</v>
       </c>
@@ -2005,7 +2210,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" ht="18">
+    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>159</v>
       </c>
@@ -2014,98 +2219,120 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" ht="18">
+    <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" ht="18">
+    <row r="23" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:5" ht="18">
+        <v>372</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:5" ht="18">
+    <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="18">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="18">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="18">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="18">
-      <c r="A29" s="3" t="s">
+      <c r="B28" s="7" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A30" s="3" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A31" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A32" s="3" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="18" x14ac:dyDescent="0.45">
+      <c r="A33" s="1" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="18">
-      <c r="A30" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="B30" s="2" t="s">
+    <row r="34" spans="1:2" ht="18" x14ac:dyDescent="0.45">
+      <c r="A34" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="18">
-      <c r="A31" s="3" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="10" t="s">
+    <row r="35" spans="1:2" ht="18" x14ac:dyDescent="0.45">
+      <c r="A35" s="1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="10" t="s">
+    <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="18">
-      <c r="A34" s="10" t="s">
+    <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.45">
+      <c r="A38" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="10" t="s">
+    <row r="39" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="8"/>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2129,18 +2356,29 @@
     <hyperlink ref="B12" location="'تمرین فصل 3'!A1" display="تمرین فصل 3"/>
     <hyperlink ref="B15" location="'تمرین فصل 4'!A1" display="تمرین فصل 4"/>
     <hyperlink ref="B18" location="'تمرین فصل 5'!A1" display="تمرین فصل 5"/>
-    <hyperlink ref="A19" location="'معرفی موتورها'!A1" display="معرفی موتورها"/>
-    <hyperlink ref="A20" location="'موتور دی سی یک'!A1" display="موتور دی سی یک"/>
-    <hyperlink ref="A21" location="'موتور دی سی دو'!A1" display="موتور دی سی دو"/>
-    <hyperlink ref="A22" location="سرو!A1" display="سرو"/>
-    <hyperlink ref="A23" location="استپ!A1" display="استپر موتور"/>
-    <hyperlink ref="A24" location="براشلس!A1" display="براشلس"/>
-    <hyperlink ref="A25" location="'فاصله سنجی'!A1" display="فاصله سنجی "/>
-    <hyperlink ref="A31" location="'حافظه دائمی'!A1" display="حافظه دائمی"/>
+    <hyperlink ref="A19" location="'16 معرفی موتورها'!A1" display="معرفی موتورها"/>
+    <hyperlink ref="A20" location="'17 موتور دی سی یک'!A1" display="موتور دی سی یک"/>
+    <hyperlink ref="A21" location="'18 موتور دی سی دو'!A1" display="موتور دی سی دو"/>
+    <hyperlink ref="A22" location="'19 سرو'!A1" display="سرو"/>
+    <hyperlink ref="A23" location="'20 استپ'!A1" display="استپر موتور"/>
+    <hyperlink ref="A24" location="'21 براشلس'!A1" display="براشلس"/>
+    <hyperlink ref="A25" location="'22 فاصله سنجی اولتراسونیک'!A1" display="فاصله سنجی اولتراسونیک"/>
     <hyperlink ref="A1" location="'پیش نیاز الکتریکی'!A1" display="پیش نیاز"/>
     <hyperlink ref="A2" location="'پیش نیاز برنامه نویسی'!A1" display="پیش نیاز برنامه نویسی"/>
     <hyperlink ref="A3" location="'مدار منطقی'!A1" display="مدار منطقی"/>
     <hyperlink ref="B3" location="'تمرین فصل 0'!A1" display="تمرین فصل 0 "/>
+    <hyperlink ref="A34" location="' 31 EEPROM'!A1" display="EEPROM"/>
+    <hyperlink ref="A30" location="'آی سی ساعت'!A1" display="آی سی ساعت"/>
+    <hyperlink ref="A29" location="I2C!A1" display="I2C"/>
+    <hyperlink ref="B23" location="'تمرین فصل 6'!A1" display="تمرین فصل 6"/>
+    <hyperlink ref="A26" location="'23 فاصله سنجی آی آر'!A1" display="فاصله سنجی آی آر"/>
+    <hyperlink ref="A27" location="'24 شافت انکودر'!A1" display="شافت انکودر"/>
+    <hyperlink ref="A28" location="'25 روتاری انکودر'!A1" display="روتاری انکودر"/>
+    <hyperlink ref="B28" location="'تمرین فصل 7'!A1" display="تمرین فصل 7"/>
+    <hyperlink ref="A31" location="'28 SPI'!A1" display="SPI"/>
+    <hyperlink ref="A32" location="'29 کاربرد SPI'!A1" display="قطعه کاربردی برای SPI"/>
+    <hyperlink ref="A33" location="'30 Tone'!A1" display="Tone (تولید صدا)"/>
+    <hyperlink ref="A35" location="'32 SD Card'!A1" display="SD Card"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2149,56 +2387,22 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A13"/>
+  <dimension ref="D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="1" width="80.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="85.75" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="22.5">
-      <c r="A13" s="9" t="s">
-        <v>382</v>
+    <row r="10" spans="4:4" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="D10" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A13" location="Sheet1!A1" display="صفحه اصلی"/>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2206,13 +2410,647 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D9"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="9" spans="4:4" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="D9" s="8" t="s">
+        <v>379</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E10"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="10" spans="5:5" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="E10" s="8" t="s">
+        <v>379</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E10" location="Sheet1!A1" display="صفحه اصلی"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="C8" s="8" t="s">
+        <v>379</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C8" location="Sheet1!A1" display="صفحه اصلی"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D10"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="10" spans="4:4" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="D10" s="8" t="s">
+        <v>379</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="C1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="D11" s="8" t="s">
+        <v>379</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D11" location="Sheet1!A1" display="صفحه اصلی"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13.75" customWidth="1"/>
+    <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="C2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="D3" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="D10" s="8" t="s">
+        <v>379</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="D9" s="8" t="s">
+        <v>379</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="D9" s="8" t="s">
+        <v>379</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="10" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="C10" s="8" t="s">
+        <v>379</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D10"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="10" spans="4:4" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="D10" s="8" t="s">
+        <v>379</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="12" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="D12" s="8" t="s">
+        <v>379</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D12" location="Sheet1!A1" display="صفحه اصلی"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="80.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="85.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>379</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A13" location="Sheet1!A1" display="صفحه اصلی"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
@@ -2221,34 +3059,37 @@
     <col min="5" max="5" width="51.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="E1" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>328</v>
-      </c>
-      <c r="B2" t="s">
-        <v>330</v>
-      </c>
-      <c r="E2" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="22.5">
-      <c r="C9" s="9" t="s">
-        <v>382</v>
+    </row>
+    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="C9" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -2259,7 +3100,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
@@ -2267,7 +3108,7 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.25" customWidth="1"/>
     <col min="2" max="2" width="19.75" customWidth="1"/>
@@ -2275,7 +3116,7 @@
     <col min="4" max="4" width="24.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -2289,7 +3130,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>297</v>
       </c>
@@ -2300,7 +3141,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>298</v>
       </c>
@@ -2308,14 +3149,14 @@
         <v>304</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22.5">
-      <c r="C11" s="9" t="s">
-        <v>382</v>
+    <row r="11" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="C11" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -2326,7 +3167,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
@@ -2334,7 +3175,7 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.125" customWidth="1"/>
     <col min="2" max="2" width="27.875" bestFit="1" customWidth="1"/>
@@ -2345,80 +3186,87 @@
     <col min="7" max="7" width="32.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B3" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="C1" t="s">
-        <v>361</v>
-      </c>
-      <c r="D1" t="s">
-        <v>364</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="C3" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="F1" t="s">
-        <v>366</v>
-      </c>
-      <c r="G1" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
+      <c r="E3" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="B2" t="s">
-        <v>353</v>
-      </c>
-      <c r="C2" t="s">
-        <v>362</v>
-      </c>
-      <c r="D2" t="s">
-        <v>358</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="F2" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>350</v>
-      </c>
-      <c r="B3" t="s">
-        <v>354</v>
-      </c>
-      <c r="C3" t="s">
-        <v>363</v>
-      </c>
-      <c r="D3" t="s">
-        <v>359</v>
-      </c>
-      <c r="E3" t="s">
-        <v>365</v>
-      </c>
-      <c r="F3" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>351</v>
-      </c>
-      <c r="D4" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="22.5">
-      <c r="B11" s="9" t="s">
-        <v>382</v>
+      <c r="E4" s="4"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="E5" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="B11" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -2429,7 +3277,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A11"/>
   <sheetViews>
@@ -2437,45 +3285,45 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="75" customWidth="1"/>
     <col min="2" max="2" width="64.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="22.5">
-      <c r="A11" s="9" t="s">
-        <v>382</v>
+    <row r="11" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -2486,7 +3334,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -2494,7 +3342,7 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.75" customWidth="1"/>
@@ -2503,33 +3351,33 @@
     <col min="5" max="5" width="25.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>334</v>
       </c>
-      <c r="B1" t="s">
-        <v>337</v>
-      </c>
-      <c r="C1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>335</v>
-      </c>
-      <c r="B2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="22.5">
-      <c r="C9" s="9" t="s">
-        <v>382</v>
+    </row>
+    <row r="9" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="C9" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -2540,7 +3388,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
@@ -2548,7 +3396,7 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="26.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="28.125" style="2" bestFit="1" customWidth="1"/>
@@ -2559,7 +3407,7 @@
     <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>267</v>
       </c>
@@ -2576,7 +3424,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>291</v>
       </c>
@@ -2593,7 +3441,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>276</v>
       </c>
@@ -2604,10 +3452,10 @@
         <v>289</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>277</v>
       </c>
@@ -2615,52 +3463,52 @@
         <v>290</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B11" s="2" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B12" s="2" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="22.5">
-      <c r="C15" s="9" t="s">
-        <v>382</v>
+    <row r="15" spans="1:5" ht="22.5" x14ac:dyDescent="0.45">
+      <c r="C15" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -2671,7 +3519,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -2679,7 +3527,7 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="17.875" style="2" customWidth="1"/>
@@ -2689,7 +3537,7 @@
     <col min="6" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>270</v>
       </c>
@@ -2706,7 +3554,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -2717,7 +3565,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>261</v>
       </c>
@@ -2725,14 +3573,14 @@
         <v>265</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="22.5">
-      <c r="C10" s="9" t="s">
-        <v>382</v>
+    <row r="10" spans="1:5" ht="22.5" x14ac:dyDescent="0.45">
+      <c r="C10" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -2744,7 +3592,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -2752,14 +3600,14 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="44.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="22.5">
+    <row r="1" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>240</v>
       </c>
@@ -2767,45 +3615,45 @@
         <v>241</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="22.5">
+    <row r="2" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
         <v>242</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:2" ht="22.5">
+    <row r="3" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6" t="s">
         <v>246</v>
       </c>
       <c r="B3" s="6"/>
     </row>
-    <row r="4" spans="1:2" ht="22.5">
+    <row r="4" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6" t="s">
         <v>243</v>
       </c>
       <c r="B4" s="6"/>
     </row>
-    <row r="5" spans="1:2" ht="22.5">
+    <row r="5" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="6" t="s">
         <v>247</v>
       </c>
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="1:2" ht="22.5">
+    <row r="6" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="6" t="s">
         <v>244</v>
       </c>
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:2" ht="22.5">
+    <row r="7" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="6" t="s">
         <v>245</v>
       </c>
       <c r="B7" s="6"/>
     </row>
-    <row r="9" spans="1:2" ht="22.5">
-      <c r="B9" s="9" t="s">
-        <v>382</v>
+    <row r="9" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="B9" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -2817,7 +3665,79 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B5" s="13" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B6" s="13" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="C9" s="8" t="s">
+        <v>379</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -2825,7 +3745,7 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="26.375" style="2" customWidth="1"/>
     <col min="2" max="2" width="31.875" style="2" customWidth="1"/>
@@ -2835,7 +3755,7 @@
     <col min="6" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>223</v>
       </c>
@@ -2849,7 +3769,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>224</v>
       </c>
@@ -2863,7 +3783,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>227</v>
       </c>
@@ -2871,44 +3791,44 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="22.5">
-      <c r="B13" s="9" t="s">
-        <v>382</v>
+    <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.45">
+      <c r="B13" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -2919,80 +3839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
-  <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.75" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="24">
-      <c r="A1" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="24">
-      <c r="A2" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="24">
-      <c r="A3" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="24">
-      <c r="A4" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="20.25">
-      <c r="B5" s="7" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="20.25">
-      <c r="B6" s="7" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="22.5">
-      <c r="C9" s="9" t="s">
-        <v>382</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -3000,7 +3847,7 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.5" customWidth="1"/>
     <col min="2" max="2" width="25.875" bestFit="1" customWidth="1"/>
@@ -3008,7 +3855,7 @@
     <col min="4" max="4" width="46.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>210</v>
       </c>
@@ -3019,10 +3866,10 @@
         <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>211</v>
       </c>
@@ -3033,7 +3880,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>212</v>
       </c>
@@ -3041,14 +3888,14 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="22.5">
-      <c r="B13" s="9" t="s">
-        <v>382</v>
+    <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="B13" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -3059,7 +3906,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -3067,7 +3914,7 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14.375" style="2" customWidth="1"/>
     <col min="2" max="2" width="18.25" style="2" customWidth="1"/>
@@ -3078,7 +3925,7 @@
     <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>112</v>
       </c>
@@ -3098,7 +3945,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>196</v>
       </c>
@@ -3115,7 +3962,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>209</v>
       </c>
@@ -3129,7 +3976,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>200</v>
       </c>
@@ -3137,14 +3984,14 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D5" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="22.5">
-      <c r="B13" s="9" t="s">
-        <v>382</v>
+    <row r="13" spans="1:6" ht="22.5" x14ac:dyDescent="0.45">
+      <c r="B13" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -3155,7 +4002,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -3163,21 +4010,21 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.75" customWidth="1"/>
     <col min="2" max="2" width="17.875" customWidth="1"/>
     <col min="3" max="3" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="22.5">
-      <c r="B6" s="9" t="s">
-        <v>382</v>
+    <row r="6" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="B6" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -3188,7 +4035,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
@@ -3196,7 +4043,7 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.625" customWidth="1"/>
@@ -3206,7 +4053,7 @@
     <col min="7" max="7" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>133</v>
       </c>
@@ -3229,7 +4076,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -3243,29 +4090,29 @@
         <v>251</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="22.5">
-      <c r="B13" s="9" t="s">
-        <v>382</v>
+    <row r="13" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="B13" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -3276,7 +4123,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
@@ -3284,7 +4131,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
@@ -3293,7 +4140,7 @@
     <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>112</v>
       </c>
@@ -3310,7 +4157,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>113</v>
       </c>
@@ -3325,7 +4172,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="18">
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>114</v>
       </c>
@@ -3340,7 +4187,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="18">
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>115</v>
       </c>
@@ -3353,7 +4200,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="18">
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>116</v>
       </c>
@@ -3364,9 +4211,9 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="22.5">
-      <c r="C13" s="9" t="s">
-        <v>382</v>
+    <row r="13" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="C13" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -3377,7 +4224,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -3385,7 +4232,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
@@ -3393,7 +4240,7 @@
     <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>146</v>
       </c>
@@ -3407,7 +4254,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>147</v>
       </c>
@@ -3421,19 +4268,19 @@
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="22.5">
-      <c r="C13" s="9" t="s">
-        <v>382</v>
+    <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="C13" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -3445,7 +4292,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -3453,19 +4300,19 @@
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="22.5">
-      <c r="B7" s="9" t="s">
-        <v>382</v>
+    <row r="7" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="B7" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -3476,7 +4323,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
@@ -3484,7 +4331,7 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="23.375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.375" style="2" customWidth="1"/>
@@ -3496,7 +4343,7 @@
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>160</v>
       </c>
@@ -3510,7 +4357,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>85</v>
       </c>
@@ -3524,7 +4371,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>86</v>
       </c>
@@ -3535,7 +4382,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C4" s="2" t="s">
         <v>106</v>
       </c>
@@ -3543,7 +4390,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C5" s="2" t="s">
         <v>107</v>
       </c>
@@ -3551,14 +4398,14 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C6" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22.5">
-      <c r="B11" s="9" t="s">
-        <v>382</v>
+    <row r="11" spans="1:4" ht="22.5" x14ac:dyDescent="0.45">
+      <c r="B11" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -3570,7 +4417,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -3578,7 +4425,7 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.25" customWidth="1"/>
@@ -3587,7 +4434,7 @@
     <col min="5" max="5" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>123</v>
       </c>
@@ -3601,7 +4448,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>124</v>
       </c>
@@ -3615,7 +4462,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>125</v>
       </c>
@@ -3629,7 +4476,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>129</v>
@@ -3641,7 +4488,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18">
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>69</v>
@@ -3649,9 +4496,9 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="22.5">
-      <c r="B13" s="9" t="s">
-        <v>382</v>
+    <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="B13" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -3662,7 +4509,58 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
+      <c r="A1" s="12" t="s">
+        <v>439</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
+      <c r="A2" s="12" t="s">
+        <v>440</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
+      <c r="A3" s="12" t="s">
+        <v>441</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+    </row>
+    <row r="7" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="D7" s="8" t="s">
+        <v>379</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D7" location="Sheet1!A1" display="صفحه اصلی"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
@@ -3670,7 +4568,7 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.875" style="2" bestFit="1" customWidth="1"/>
@@ -3682,7 +4580,7 @@
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
@@ -3705,7 +4603,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="D2" s="2" t="s">
         <v>55</v>
       </c>
@@ -3719,7 +4617,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E3" s="2" t="s">
         <v>57</v>
       </c>
@@ -3730,7 +4628,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E4" s="2" t="s">
         <v>58</v>
       </c>
@@ -3741,7 +4639,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E5" s="2" t="s">
         <v>59</v>
       </c>
@@ -3750,21 +4648,21 @@
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="F6" s="4" t="s">
         <v>65</v>
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="F7" s="4" t="s">
         <v>66</v>
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="22.5">
-      <c r="C10" s="9" t="s">
-        <v>382</v>
+    <row r="10" spans="1:7" ht="22.5" x14ac:dyDescent="0.45">
+      <c r="C10" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -3775,78 +4673,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView rightToLeft="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.75" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="18">
-      <c r="A1" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="C1" t="s">
-        <v>314</v>
-      </c>
-      <c r="D1" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="18">
-      <c r="A2" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="C2" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18">
-      <c r="A3" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="C3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="C4" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="22.5">
-      <c r="C8" s="9" t="s">
-        <v>382</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C8" location="Sheet1!A1" display="صفحه اصلی"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -3854,19 +4681,19 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="22.5">
-      <c r="C4" s="9" t="s">
-        <v>382</v>
+    <row r="4" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="C4" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -3877,7 +4704,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
@@ -3885,12 +4712,12 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -3919,7 +4746,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>94</v>
       </c>
@@ -3927,7 +4754,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -3935,9 +4762,9 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="22.5">
-      <c r="G7" s="9" t="s">
-        <v>382</v>
+    <row r="7" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="G7" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -3948,7 +4775,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -3956,9 +4783,9 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>254</v>
       </c>
@@ -3966,7 +4793,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>249</v>
       </c>
@@ -3974,7 +4801,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>255</v>
       </c>
@@ -3982,7 +4809,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>256</v>
       </c>
@@ -3990,9 +4817,9 @@
         <v>259</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="22.5">
-      <c r="D9" s="9" t="s">
-        <v>382</v>
+    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="D9" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -4003,70 +4830,48 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5">
-      <c r="A1" s="9" t="s">
-        <v>382</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:5" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="22.5">
-      <c r="E9" s="9" t="s">
-        <v>382</v>
+    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="E9" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="Sheet1!A1" display="صفحه اصلی"/>
     <hyperlink ref="E9" location="Sheet1!A1" display="صفحه اصلی"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D11"/>
-  <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData>
-    <row r="11" spans="4:4" ht="22.5">
-      <c r="D11" s="9" t="s">
-        <v>382</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D11" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4074,17 +4879,94 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D10"/>
+  <dimension ref="D7"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="7" spans="4:4" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="D7" s="8" t="s">
+        <v>379</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D7" location="Sheet1!A1" display="صفحه اصلی"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="10" spans="4:4" ht="22.5">
-      <c r="D10" s="9" t="s">
-        <v>382</v>
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="B2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="B4" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="D10" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -4095,116 +4977,48 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="22.5">
-      <c r="D9" s="9" t="s">
-        <v>382</v>
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.45">
+      <c r="A1" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="C6" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
-  <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="1" width="11.875" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="22.5">
-      <c r="D9" s="9" t="s">
-        <v>382</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
+    <hyperlink ref="C6" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4212,65 +5026,78 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A4" sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.125" customWidth="1"/>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="18">
+        <v>404</v>
+      </c>
+      <c r="B1" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" ht="18">
+        <v>405</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" ht="18">
+        <v>177</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="10" spans="1:3" ht="22.5">
-      <c r="C10" s="9" t="s">
-        <v>382</v>
+        <v>406</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="11" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="E9" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی"/>
+    <hyperlink ref="E9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4278,71 +5105,22 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="D9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="1" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.25" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="B2" t="s">
-        <v>188</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="B3" t="s">
-        <v>189</v>
-      </c>
-      <c r="C3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="B4" t="s">
-        <v>190</v>
-      </c>
-      <c r="C4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="22.5">
-      <c r="D12" s="9" t="s">
-        <v>382</v>
+    <row r="9" spans="4:4" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="D9" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D12" location="Sheet1!A1" display="صفحه اصلی"/>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>